<commit_message>
Fixed severe link conflict
</commit_message>
<xml_diff>
--- a/elective_datasheet.xlsx
+++ b/elective_datasheet.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANISH\Documents\project_stuff\wt2_project\WT2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="510" yWindow="570" windowWidth="14055" windowHeight="4050"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="129">
   <si>
     <t>Elective_no</t>
   </si>
@@ -404,12 +409,15 @@
   <si>
     <t>Interests</t>
   </si>
+  <si>
+    <t>Dr. Antony Priyakumar</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -489,6 +497,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -535,7 +551,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -567,9 +583,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -601,6 +618,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -776,17 +794,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
     <col min="3" max="3" width="48.7109375" customWidth="1"/>
@@ -794,7 +812,7 @@
     <col min="5" max="6" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -818,7 +836,7 @@
       </c>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -842,7 +860,7 @@
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -866,7 +884,7 @@
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -890,7 +908,7 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -914,7 +932,7 @@
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -938,7 +956,7 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -962,7 +980,7 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -986,7 +1004,7 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -1010,7 +1028,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -1034,7 +1052,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -1058,7 +1076,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -1082,7 +1100,7 @@
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>3</v>
       </c>
@@ -1106,7 +1124,7 @@
       </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>3</v>
       </c>
@@ -1130,7 +1148,7 @@
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -1154,7 +1172,7 @@
       </c>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -1178,7 +1196,7 @@
       </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>3</v>
       </c>
@@ -1189,7 +1207,7 @@
         <v>66</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>67</v>
+        <v>128</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>48</v>
@@ -1202,7 +1220,7 @@
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>4</v>
       </c>
@@ -1226,7 +1244,7 @@
       </c>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>4</v>
       </c>
@@ -1250,7 +1268,7 @@
       </c>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>4</v>
       </c>
@@ -1274,7 +1292,7 @@
       </c>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>4</v>
       </c>
@@ -1298,7 +1316,7 @@
       </c>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>4</v>
       </c>
@@ -1322,7 +1340,7 @@
       </c>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1">
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>4</v>
       </c>
@@ -1346,7 +1364,7 @@
       </c>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>5</v>
       </c>
@@ -1370,7 +1388,7 @@
       </c>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>5</v>
       </c>
@@ -1394,7 +1412,7 @@
       </c>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>5</v>
       </c>
@@ -1418,7 +1436,7 @@
       </c>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1">
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>5</v>
       </c>
@@ -1442,7 +1460,7 @@
       </c>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1">
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>5</v>
       </c>
@@ -1466,7 +1484,7 @@
       </c>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1">
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>5</v>
       </c>
@@ -1490,7 +1508,7 @@
       </c>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1">
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>6</v>
       </c>
@@ -1514,7 +1532,7 @@
       </c>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1">
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>6</v>
       </c>
@@ -1538,7 +1556,7 @@
       </c>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1">
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>6</v>
       </c>
@@ -1562,7 +1580,7 @@
       </c>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" ht="15.75" customHeight="1">
+    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>6</v>
       </c>
@@ -1586,7 +1604,7 @@
       </c>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" ht="15.75" customHeight="1">
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>6</v>
       </c>
@@ -1610,7 +1628,7 @@
       </c>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" ht="15.75" customHeight="1">
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>6</v>
       </c>
@@ -1634,7 +1652,7 @@
       </c>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" ht="15.75" customHeight="1">
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>6</v>
       </c>
@@ -1658,7 +1676,7 @@
       </c>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" ht="15.75" customHeight="1">
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>7</v>
       </c>
@@ -1682,7 +1700,7 @@
       </c>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" ht="15.75" customHeight="1">
+    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>7</v>
       </c>
@@ -1706,7 +1724,7 @@
       </c>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="15.75" customHeight="1">
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>7</v>
       </c>
@@ -1730,7 +1748,7 @@
       </c>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" ht="15.75" customHeight="1">
+    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>7</v>
       </c>

</xml_diff>